<commit_message>
Updated Y for VSP-Payments-Data.
</commit_message>
<xml_diff>
--- a/KatalonData/Bootstrap/VSP-Payments-Data.xlsx
+++ b/KatalonData/Bootstrap/VSP-Payments-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E6FFD1-F12B-4301-9B7C-1A0503DD5465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7411ED3-C785-40CC-9293-E17F30F37E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="2835" windowWidth="21600" windowHeight="12735" activeTab="2" xr2:uid="{8EA648C6-9B74-4918-B9F6-8ECD80D98AD5}"/>
+    <workbookView xWindow="-27540" yWindow="210" windowWidth="16455" windowHeight="17160" activeTab="1" xr2:uid="{8EA648C6-9B74-4918-B9F6-8ECD80D98AD5}"/>
   </bookViews>
   <sheets>
     <sheet name="CC-Payments-Sale" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="88">
   <si>
     <t>Result</t>
   </si>
@@ -2421,6 +2421,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2428,8 +2431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1343EF54-4827-416A-A016-C445805C86F0}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="42.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,6 +2614,9 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2676,6 +2682,9 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
@@ -2741,6 +2750,9 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
@@ -2806,6 +2818,9 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2871,6 +2886,9 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2936,6 +2954,9 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
@@ -3001,6 +3022,9 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
@@ -3134,6 +3158,9 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>62</v>
       </c>
@@ -3199,6 +3226,9 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>62</v>
       </c>
@@ -3264,6 +3294,9 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>62</v>
       </c>
@@ -3329,6 +3362,9 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>62</v>
       </c>
@@ -3394,6 +3430,9 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>62</v>
       </c>
@@ -3459,6 +3498,9 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>62</v>
       </c>
@@ -3524,6 +3566,9 @@
       </c>
     </row>
     <row r="17" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>62</v>
       </c>
@@ -3657,6 +3702,9 @@
       </c>
     </row>
     <row r="19" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>66</v>
       </c>
@@ -3722,6 +3770,9 @@
       </c>
     </row>
     <row r="20" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>66</v>
       </c>
@@ -3787,6 +3838,9 @@
       </c>
     </row>
     <row r="21" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>66</v>
       </c>
@@ -3852,6 +3906,9 @@
       </c>
     </row>
     <row r="22" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E22" s="1" t="s">
         <v>66</v>
       </c>
@@ -3917,6 +3974,9 @@
       </c>
     </row>
     <row r="23" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>66</v>
       </c>
@@ -3982,6 +4042,9 @@
       </c>
     </row>
     <row r="24" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>66</v>
       </c>
@@ -4047,6 +4110,9 @@
       </c>
     </row>
     <row r="25" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E25" s="1" t="s">
         <v>66</v>
       </c>
@@ -4113,6 +4179,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -4120,7 +4189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B3AC86-4723-49D7-AB53-411E6A25C44B}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D16"/>
     </sheetView>
   </sheetViews>
@@ -5220,5 +5289,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>